<commit_message>
feat: histograms of temperature distribution
</commit_message>
<xml_diff>
--- a/data/1.5T/thermometry_analysis_Method.REGIONWISE_BOOTSTRAP.xlsx
+++ b/data/1.5T/thermometry_analysis_Method.REGIONWISE_BOOTSTRAP.xlsx
@@ -480,10 +480,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>15.09251810730188</v>
+        <v>15.0677871054159</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8949084889538171</v>
+        <v>0.8086528589963745</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -500,10 +500,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>13.28792154272096</v>
+        <v>13.65273615994774</v>
       </c>
       <c r="E3" t="n">
-        <v>1.852003383303082</v>
+        <v>2.056412934489027</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
@@ -520,10 +520,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>15.89272019141352</v>
+        <v>15.84884973754504</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5053240561022281</v>
+        <v>0.4737798588840921</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -540,10 +540,10 @@
         <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>14.57900706373723</v>
+        <v>14.82296216149963</v>
       </c>
       <c r="E5" t="n">
-        <v>1.317536999549197</v>
+        <v>1.470271652439198</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
@@ -560,10 +560,10 @@
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>16.24907194954956</v>
+        <v>16.27049478550594</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5639013858380321</v>
+        <v>0.5175175310755836</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
@@ -580,10 +580,10 @@
         <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>15.20183071024991</v>
+        <v>15.36140106242473</v>
       </c>
       <c r="E7" t="n">
-        <v>1.053083464862801</v>
+        <v>1.160568058301429</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
@@ -600,10 +600,10 @@
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>16.28126850077917</v>
+        <v>16.27619821733979</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5405018338101529</v>
+        <v>0.4962008151841023</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -620,10 +620,10 @@
         <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>15.41732941218705</v>
+        <v>15.48154308277698</v>
       </c>
       <c r="E9" t="n">
-        <v>0.766611697958401</v>
+        <v>0.7801327716119801</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
@@ -640,10 +640,10 @@
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>16.74260463746512</v>
+        <v>16.82246103450655</v>
       </c>
       <c r="E10" t="n">
-        <v>0.467936357338787</v>
+        <v>0.521185082417052</v>
       </c>
       <c r="F10" t="n">
         <v>1</v>
@@ -660,10 +660,10 @@
         <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>16.09103560045649</v>
+        <v>16.13016089284572</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9095294389632181</v>
+        <v>0.8896458082423097</v>
       </c>
       <c r="F11" t="n">
         <v>1</v>
@@ -680,10 +680,10 @@
         <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>20.30739905821708</v>
+        <v>20.04140488260402</v>
       </c>
       <c r="E12" t="n">
-        <v>2.157164194910536</v>
+        <v>2.00159589401732</v>
       </c>
       <c r="F12" t="n">
         <v>1</v>
@@ -700,10 +700,10 @@
         <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>17.26918677085792</v>
+        <v>17.34250682055415</v>
       </c>
       <c r="E13" t="n">
-        <v>0.4839862706539249</v>
+        <v>0.5344189831229733</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
@@ -720,10 +720,10 @@
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>21.2240955428253</v>
+        <v>20.93593117027743</v>
       </c>
       <c r="E14" t="n">
-        <v>2.803685522133372</v>
+        <v>2.659476564274648</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
@@ -740,10 +740,10 @@
         <v>2</v>
       </c>
       <c r="D15" t="n">
-        <v>17.50305633939872</v>
+        <v>17.63861984181357</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9116261520379708</v>
+        <v>1.00072081656106</v>
       </c>
       <c r="F15" t="n">
         <v>1</v>
@@ -760,10 +760,10 @@
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>22.11523112319985</v>
+        <v>21.80860802039622</v>
       </c>
       <c r="E16" t="n">
-        <v>2.767182637711156</v>
+        <v>2.621958038061083</v>
       </c>
       <c r="F16" t="n">
         <v>1</v>
@@ -780,10 +780,10 @@
         <v>2</v>
       </c>
       <c r="D17" t="n">
-        <v>17.2644258099164</v>
+        <v>17.41312086157644</v>
       </c>
       <c r="E17" t="n">
-        <v>1.002099950961893</v>
+        <v>1.098932289689143</v>
       </c>
       <c r="F17" t="n">
         <v>1</v>
@@ -800,10 +800,10 @@
         <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>22.4586077495038</v>
+        <v>22.07572639411203</v>
       </c>
       <c r="E18" t="n">
-        <v>2.843325068529555</v>
+        <v>2.706390963726625</v>
       </c>
       <c r="F18" t="n">
         <v>1</v>
@@ -820,10 +820,10 @@
         <v>2</v>
       </c>
       <c r="D19" t="n">
-        <v>18.05670832847533</v>
+        <v>18.18954593210566</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9268877738886904</v>
+        <v>1.014170911387849</v>
       </c>
       <c r="F19" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
feat: updated results for abstract
</commit_message>
<xml_diff>
--- a/data/1.5T/thermometry_analysis_Method.REGIONWISE_BOOTSTRAP.xlsx
+++ b/data/1.5T/thermometry_analysis_Method.REGIONWISE_BOOTSTRAP.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,6 +468,16 @@
           <t>interval</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>num_samples</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>fractional_uncertainty</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -488,6 +498,12 @@
       <c r="F2" t="n">
         <v>1</v>
       </c>
+      <c r="G2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.05465967198530568</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -508,6 +524,12 @@
       <c r="F3" t="n">
         <v>1</v>
       </c>
+      <c r="G3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.1517863286558169</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -528,6 +550,12 @@
       <c r="F4" t="n">
         <v>1</v>
       </c>
+      <c r="G4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.03076134861937979</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -547,6 +575,12 @@
       </c>
       <c r="F5" t="n">
         <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.1002143141730702</v>
       </c>
     </row>
     <row r="6">
@@ -568,6 +602,12 @@
       <c r="F6" t="n">
         <v>1</v>
       </c>
+      <c r="G6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.03284310601598622</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -588,6 +628,12 @@
       <c r="F7" t="n">
         <v>1</v>
       </c>
+      <c r="G7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.07607541391771377</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -608,6 +654,12 @@
       <c r="F8" t="n">
         <v>1</v>
       </c>
+      <c r="G8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.03160184766307855</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -628,6 +680,12 @@
       <c r="F9" t="n">
         <v>1</v>
       </c>
+      <c r="G9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.05038480137631279</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -648,6 +706,12 @@
       <c r="F10" t="n">
         <v>1</v>
       </c>
+      <c r="G10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.03108241073896207</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -668,6 +732,12 @@
       <c r="F11" t="n">
         <v>1</v>
       </c>
+      <c r="G11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.05481633040125691</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -688,6 +758,12 @@
       <c r="F12" t="n">
         <v>1</v>
       </c>
+      <c r="G12" t="n">
+        <v>993</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.1057280547432848</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -708,6 +784,12 @@
       <c r="F13" t="n">
         <v>1</v>
       </c>
+      <c r="G13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.03084771414731377</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -728,6 +810,12 @@
       <c r="F14" t="n">
         <v>1</v>
       </c>
+      <c r="G14" t="n">
+        <v>988</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.1337567131970655</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -748,6 +836,12 @@
       <c r="F15" t="n">
         <v>1</v>
       </c>
+      <c r="G15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.05682149308062914</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -768,6 +862,12 @@
       <c r="F16" t="n">
         <v>1</v>
       </c>
+      <c r="G16" t="n">
+        <v>999</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.127338086543459</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -788,6 +888,12 @@
       <c r="F17" t="n">
         <v>1</v>
       </c>
+      <c r="G17" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.06317416027103828</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -808,6 +914,12 @@
       <c r="F18" t="n">
         <v>1</v>
       </c>
+      <c r="G18" t="n">
+        <v>995</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.1301786259478235</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -827,6 +939,12 @@
       </c>
       <c r="F19" t="n">
         <v>1</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.05576595618402488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>